<commit_message>
Update README.md, queryLLM.py, and requirements.txt to streamline dependencies and remove unused imports
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -548,7 +548,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor README.md for clarity, enhance queryLLM.py with structured response handling, and update requirements.txt to reflect dependencies. Add test and trial Excel files for validation.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>response</t>
+          <t>verdict</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -473,11 +473,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9">
@@ -563,11 +563,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10">
@@ -597,8 +597,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.8</v>
-      </c>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>The name of my grandfather is John</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>INSUFFICIENT INFO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Enhance README.md with virtual environment setup instructions, update queryLLM.py to set temperature for client.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5">
@@ -503,11 +503,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="9">
@@ -563,11 +563,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Refactor queryLLM.py to enhance fact-checking prompts and system instructions; remove unnecessary lock file.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -458,12 +458,10 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.7</v>
-      </c>
+          <t>INSUFFICIENT INFO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -473,11 +471,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -488,12 +486,10 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.9</v>
-      </c>
+          <t>INSUFFICIENT INFO</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -507,7 +503,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -548,12 +544,10 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.8</v>
-      </c>
+          <t>INSUFFICIENT INFO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -563,12 +557,10 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
+          <t>INSUFFICIENT INFO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -597,7 +589,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="12">
@@ -608,10 +600,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>INSUFFICIENT INFO</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add connection testing for Ollama client and handle errors gracefully
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -458,10 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>INSUFFICIENT INFO</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -471,11 +473,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -486,10 +488,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>INSUFFICIENT INFO</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -503,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6">
@@ -514,7 +518,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -557,10 +561,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>INSUFFICIENT INFO</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -589,7 +595,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -600,12 +606,10 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
+          <t>INSUFFICIENT INFO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add field validator for verdict normalization in Truth model
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -518,12 +518,10 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.8</v>
-      </c>
+          <t>INSUFFICIENT INFO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -548,10 +546,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>INSUFFICIENT INFO</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.9333333333333333</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -561,11 +561,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -576,12 +576,10 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
+          <t>INSUFFICIENT INFO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -595,7 +593,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="12">

</xml_diff>